<commit_message>
get audio credit and share working
</commit_message>
<xml_diff>
--- a/data_tools/src/data.xlsx
+++ b/data_tools/src/data.xlsx
@@ -12,75 +12,99 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+  <si>
+    <t>head</t>
+  </si>
+  <si>
+    <t>body</t>
+  </si>
+  <si>
+    <t>yt_id</t>
+  </si>
+  <si>
+    <t>audio</t>
+  </si>
+  <si>
+    <t>audio_file</t>
+  </si>
+  <si>
+    <t>audio_credit</t>
+  </si>
+  <si>
+    <t>The Maryland National Guard arrives to help keep the piece in the wake of riots in Baltimore.</t>
+  </si>
+  <si>
+    <t>r2P3JT4Z48w</t>
+  </si>
+  <si>
+    <t>Firefighters fight a fire set by looters at a CVS store in Baltimore.</t>
+  </si>
+  <si>
+    <t>ZeHkzbWpb70</t>
+  </si>
+  <si>
+    <t>Protestors clash with police during the Baltimore riots.</t>
+  </si>
+  <si>
+    <t>cg5N4wVl2QM</t>
+  </si>
+  <si>
+    <t>An elder-care community center being built by the Southern Baptist Church burns in Baltimore.</t>
+  </si>
+  <si>
+    <t>VweR4RWrGFo</t>
+  </si>
+  <si>
+    <t>PastorDanteHickman</t>
+  </si>
+  <si>
+    <t>Pastor Dante Hickman, Southern Baptist Church</t>
+  </si>
+  <si>
+    <t>Cars burn as protestors taunt police during the Baltimore riots</t>
+  </si>
+  <si>
+    <t>i7aDNy41pUw</t>
+  </si>
   <si>
     <t>project_head</t>
   </si>
   <si>
-    <t>head</t>
+    <t>chatter</t>
   </si>
   <si>
     <t>project_share</t>
   </si>
   <si>
-    <t>body</t>
-  </si>
-  <si>
-    <t>yt_id</t>
-  </si>
-  <si>
-    <t>audio</t>
-  </si>
-  <si>
-    <t>audio_file</t>
-  </si>
-  <si>
-    <t>Baltimore Unrest</t>
-  </si>
-  <si>
-    <t>NationalGuard</t>
-  </si>
-  <si>
-    <t>Share language here</t>
-  </si>
-  <si>
-    <t>National guard footage</t>
-  </si>
-  <si>
-    <t>r2P3JT4Z48w</t>
-  </si>
-  <si>
-    <t>PastorDanteHickman</t>
-  </si>
-  <si>
-    <t>Protesters Clash</t>
-  </si>
-  <si>
-    <t>cg5N4wVl2QM</t>
-  </si>
-  <si>
-    <t>Community Center Burning</t>
-  </si>
-  <si>
-    <t>Community Center</t>
-  </si>
-  <si>
-    <t>VweR4RWrGFo</t>
+    <t>Baltimore tensions explode</t>
+  </si>
+  <si>
+    <t>Fires and looting followed the funeral of 25-year-old Freddie Gray, an unarmed black man in police custody.</t>
+  </si>
+  <si>
+    <t>Powerful raw videos from the Baltimore riots via @usatoday</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font/>
+    <font>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <sz val="14.0"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -91,6 +115,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFA2C4C9"/>
         <bgColor rgb="FFA2C4C9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -105,7 +135,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -114,13 +144,25 @@
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -144,18 +186,31 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="24.0"/>
+    <col customWidth="1" min="2" max="2" width="86.86"/>
+    <col customWidth="1" min="5" max="5" width="20.71"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -178,83 +233,14 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="2" max="2" width="38.57"/>
-    <col customWidth="1" min="5" max="5" width="20.71"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="4" t="b">
+      <c r="D2" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E2" s="5"/>
@@ -281,21 +267,17 @@
       <c r="Z2" s="5"/>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -319,16 +301,14 @@
       <c r="Z3" s="5"/>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="A4" s="3"/>
       <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="4" t="b">
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E4" s="5"/>
@@ -355,20 +335,22 @@
       <c r="Z4" s="5"/>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
@@ -392,9 +374,15 @@
     </row>
     <row r="6">
       <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
+      <c r="B6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="3" t="b">
+        <v>0</v>
+      </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
@@ -1093,4 +1081,92 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="37.0"/>
+    <col customWidth="1" min="2" max="2" width="55.57"/>
+    <col customWidth="1" min="3" max="3" width="28.57"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="5"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="9"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>